<commit_message>
Import of AURUM/Text-Tradition-1.2 from CPAN.
gitpan-cpan-distribution: Text-Tradition
gitpan-cpan-version:      1.2
gitpan-cpan-path:         AURUM/Text-Tradition-1.2.tar.gz
gitpan-cpan-author:       AURUM
gitpan-cpan-maturity:     released
</commit_message>
<xml_diff>
--- a/t/data/armexample.xlsx
+++ b/t/data/armexample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -24,9 +24,6 @@
     <t>Wit1</t>
   </si>
   <si>
-    <t>Wit2</t>
-  </si>
-  <si>
     <t>Wit3</t>
   </si>
   <si>
@@ -58,6 +55,27 @@
   </si>
   <si>
     <t>այսոսիկ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Sylfaen"/>
+        <family val="2"/>
+      </rPr>
+      <t>Աբ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -436,92 +454,92 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="17">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>